<commit_message>
Updated mACM based on comments
Updated mACM based on public comments and updated comments spreadsheets for further review.
</commit_message>
<xml_diff>
--- a/FHIR-R4/ITI_Comment_Form-mACM-Felhofer.xlsx
+++ b/FHIR-R4/ITI_Comment_Form-mACM-Felhofer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynn/Documents/IHE/2020/ITI/FHIR R4 updates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\IT-Infrastructure\FHIR-R4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0B26C6-9AC1-5842-BA23-BB2663BFE9CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E642D6-8F32-4FEB-BFE1-705E03D2D301}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30300" yWindow="460" windowWidth="25600" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4886" windowWidth="17906" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comment Form" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="166">
   <si>
     <t>Priority</t>
   </si>
@@ -1054,72 +1054,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">An Alert Aggregator should not return any patient information in transaction Mobile Report Alert [ITI-84] or Query for Alert Status [ITI-85] </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>unless</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">without </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">proper authentication and communications security </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>have been proven</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>.
-There are many reasonable methods of securing transactions. These security models can be layered in at the HTTP transport layer and do not modify the interoperability characteristics  defined in the mACM Profile.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">In Figure </t>
     </r>
     <r>
@@ -2177,13 +2111,85 @@
   </si>
   <si>
     <t>3.85.4.1.1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">An Alert Aggregator should not return any patient information in transaction Mobile Report Alert [ITI-84] or Query for Alert Status [ITI-85] </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="10"/>
+        <color theme="6" tint="0.79998168889431442"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>unless</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="0.79998168889431442"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="6" tint="0.79998168889431442"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">without </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="0.79998168889431442"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">proper authentication and communications security </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="10"/>
+        <color theme="6" tint="0.79998168889431442"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>have been proven</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="6" tint="0.79998168889431442"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>.
+There are many reasonable methods of securing transactions. These security models can be layered in at the HTTP transport layer and do not modify the interoperability characteristics  defined in the mACM Profile.</t>
+    </r>
+  </si>
+  <si>
+    <t>Fixed tables, but didn't change OIDs</t>
+  </si>
+  <si>
+    <t>queried?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2299,13 +2305,60 @@
       <name val="Courier New"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="6" tint="0.79998168889431442"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="10"/>
+      <color theme="6" tint="0.79998168889431442"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="6" tint="0.79998168889431442"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="0.79998168889431442"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -2402,7 +2455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2420,83 +2473,155 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2838,65 +2963,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J2"/>
+    <sheetView tabSelected="1" topLeftCell="C40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="55.5" customWidth="1"/>
-    <col min="3" max="3" width="4.33203125" style="26" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="23" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="16"/>
+    <col min="2" max="2" width="20.61328125" customWidth="1"/>
+    <col min="3" max="3" width="4.3046875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="10.4609375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="4.23046875" style="9" customWidth="1"/>
     <col min="6" max="6" width="44" customWidth="1"/>
-    <col min="7" max="7" width="49.6640625" style="20" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" customWidth="1"/>
-    <col min="9" max="9" width="5.5" customWidth="1"/>
+    <col min="7" max="7" width="49.69140625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="7.69140625" customWidth="1"/>
+    <col min="9" max="9" width="33.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:10" ht="18.45" x14ac:dyDescent="0.5">
+      <c r="A1" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-    </row>
-    <row r="2" spans="1:10" ht="269.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+    </row>
+    <row r="2" spans="1:10" ht="269.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-    </row>
-    <row r="3" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:10" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:10" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+    </row>
+    <row r="3" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:10" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="5" spans="1:10" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="16" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -2909,1118 +3034,1124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="12" customFormat="1" ht="42" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:10" s="25" customFormat="1" ht="38.6" x14ac:dyDescent="0.4">
+      <c r="A6" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="22">
         <v>293</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="12" customFormat="1" ht="126" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:10" s="21" customFormat="1" ht="115.75" x14ac:dyDescent="0.4">
+      <c r="A7" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="17">
         <v>293</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="12" customFormat="1" ht="56" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:10" s="25" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A8" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="26">
         <v>1</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="24">
         <v>4</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="24">
         <v>325</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="12" customFormat="1" ht="112" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:10" s="25" customFormat="1" ht="102.9" x14ac:dyDescent="0.4">
+      <c r="A9" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="26">
         <v>1</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="24">
         <v>371</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="12" customFormat="1" ht="98" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:10" s="25" customFormat="1" ht="102.9" x14ac:dyDescent="0.4">
+      <c r="A10" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="26">
         <v>1</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="27">
         <v>379</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="12" customFormat="1" ht="42" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:10" s="21" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A11" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="28">
         <v>1</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="19">
         <v>393</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="12" customFormat="1" ht="28" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:10" s="25" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A12" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="26">
         <v>1</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="24">
         <v>411</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="12" customFormat="1" ht="28" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:10" s="25" customFormat="1" ht="25.75" x14ac:dyDescent="0.4">
+      <c r="A13" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="26">
         <v>1</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="24">
         <v>424</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="12" customFormat="1" ht="154" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:10" s="25" customFormat="1" ht="141.44999999999999" x14ac:dyDescent="0.4">
+      <c r="A14" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="26">
         <v>1</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="24">
         <v>453</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="12" customFormat="1" ht="98" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+    <row r="15" spans="1:10" s="25" customFormat="1" ht="90" x14ac:dyDescent="0.4">
+      <c r="A15" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="26">
         <v>1</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="24">
         <v>480</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="12" customFormat="1" ht="56" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:10" s="25" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A16" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="29">
+      <c r="C16" s="26">
         <v>1</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="24">
         <v>500</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="12" customFormat="1" ht="112" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:8" s="25" customFormat="1" ht="102.9" x14ac:dyDescent="0.4">
+      <c r="A17" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="29">
+      <c r="C17" s="26">
         <v>1</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="24">
         <v>500</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="12" customFormat="1" ht="112" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:8" s="37" customFormat="1" ht="102.9" x14ac:dyDescent="0.4">
+      <c r="A18" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="29">
+      <c r="C18" s="34">
         <v>1</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="35">
         <v>42.5</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="36">
         <v>556</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="25" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A19" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="26">
+        <v>1</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="32">
+        <v>563</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="25" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A20" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="26">
+        <v>1</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="32">
+        <v>566</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="25" customFormat="1" ht="141" x14ac:dyDescent="0.4">
+      <c r="A21" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="26">
+        <v>1</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="32">
+        <v>573</v>
+      </c>
+      <c r="F21" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="25" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A22" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="26">
+        <v>1</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="32">
+        <v>577</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H22" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="12" customFormat="1" ht="42" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+    <row r="23" spans="1:8" s="21" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A23" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B23" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="29">
+      <c r="C23" s="28">
         <v>1</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="E19" s="15">
-        <v>563</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="H19" s="11" t="s">
+      <c r="D23" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" s="38">
+        <v>585</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="12" customFormat="1" ht="28" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
+    <row r="24" spans="1:8" s="41" customFormat="1" ht="84.9" x14ac:dyDescent="0.4">
+      <c r="A24" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B24" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="29">
+      <c r="C24" s="26">
         <v>1</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="E20" s="15">
-        <v>566</v>
-      </c>
-      <c r="F20" s="11" t="s">
+      <c r="D24" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="G20" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="H20" s="11" t="s">
+      <c r="E24" s="32">
+        <v>626</v>
+      </c>
+      <c r="F24" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="G24" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="H24" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="12" customFormat="1" ht="154" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+    <row r="25" spans="1:8" s="41" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A25" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B25" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="29">
+      <c r="C25" s="26">
         <v>1</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="E21" s="15">
-        <v>573</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="G21" s="11" t="s">
+      <c r="D25" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="32">
+        <v>633</v>
+      </c>
+      <c r="F25" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="G25" s="42"/>
+      <c r="H25" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="12" customFormat="1" ht="28" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+    <row r="26" spans="1:8" s="45" customFormat="1" ht="77.150000000000006" x14ac:dyDescent="0.4">
+      <c r="A26" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B26" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="29">
+      <c r="C26" s="28">
         <v>1</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" s="15">
-        <v>577</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="H22" s="11" t="s">
+      <c r="D26" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="38">
+        <v>640</v>
+      </c>
+      <c r="F26" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="44"/>
+      <c r="H26" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="12" customFormat="1" ht="42" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+    <row r="27" spans="1:8" s="41" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A27" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B27" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="29">
+      <c r="C27" s="26">
         <v>1</v>
       </c>
-      <c r="D23" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="E23" s="15">
-        <v>585</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="H23" s="11" t="s">
+      <c r="D27" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="G27" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="H27" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="75" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+    <row r="28" spans="1:8" s="45" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A28" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B28" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="29">
-        <v>1</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E24" s="15">
-        <v>626</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="H24" s="11" t="s">
+      <c r="C28" s="46">
+        <v>2</v>
+      </c>
+      <c r="D28" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="E28" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="F28" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="G28" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="H28" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
+    <row r="29" spans="1:8" s="41" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A29" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B29" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="29">
-        <v>1</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E25" s="15">
-        <v>633</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G25" s="21"/>
-      <c r="H25" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="84" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="29">
-        <v>1</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E26" s="15">
-        <v>640</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G26" s="21"/>
-      <c r="H26" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="28" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="29">
-        <v>1</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G27" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="42" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="30">
-        <v>2</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E28" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G28" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="42" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="2" t="s">
-        <v>154</v>
+      <c r="C29" s="47"/>
+      <c r="D29" s="39" t="s">
+        <v>153</v>
       </c>
       <c r="E29" s="32">
         <v>699</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="G29" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.2">
-      <c r="A30" s="10" t="s">
+    <row r="30" spans="1:8" s="41" customFormat="1" ht="56.6" x14ac:dyDescent="0.4">
+      <c r="A30" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="30">
+      <c r="C30" s="47">
         <v>2</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>117</v>
+      <c r="D30" s="39" t="s">
+        <v>116</v>
       </c>
       <c r="E30" s="32">
         <v>760</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G30" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="H30" s="11" t="s">
+      <c r="F30" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="G30" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="H30" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="75" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
+    <row r="31" spans="1:8" s="41" customFormat="1" ht="70.75" x14ac:dyDescent="0.4">
+      <c r="A31" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="30">
+      <c r="C31" s="47">
         <v>2</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>117</v>
+      <c r="D31" s="39" t="s">
+        <v>116</v>
       </c>
       <c r="E31" s="32">
         <v>760</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="G31" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="H31" s="11" t="s">
+      <c r="G31" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="H31" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="56" x14ac:dyDescent="0.2">
-      <c r="A32" s="10" t="s">
+    <row r="32" spans="1:8" s="41" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A32" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="30">
+      <c r="C32" s="47">
         <v>2</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>117</v>
+      <c r="D32" s="39" t="s">
+        <v>116</v>
       </c>
       <c r="E32" s="32">
         <v>760</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G32" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="H32" s="11" t="s">
+      <c r="F32" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="G32" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="H32" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="187" x14ac:dyDescent="0.2">
-      <c r="A33" s="10" t="s">
+    <row r="33" spans="1:9" s="41" customFormat="1" ht="179.6" x14ac:dyDescent="0.4">
+      <c r="A33" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="30">
+      <c r="C33" s="47">
         <v>2</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>117</v>
+      <c r="D33" s="39" t="s">
+        <v>116</v>
       </c>
       <c r="E33" s="32">
         <v>760</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G33" s="2" t="s">
+      <c r="F33" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="G33" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="H33" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="41" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A34" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="47">
+        <v>2</v>
+      </c>
+      <c r="D34" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="H33" s="11" t="s">
+      <c r="E34" s="32">
+        <v>771</v>
+      </c>
+      <c r="F34" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="G34" s="48"/>
+      <c r="H34" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="56" x14ac:dyDescent="0.2">
-      <c r="A34" s="10" t="s">
+    <row r="35" spans="1:9" s="41" customFormat="1" ht="64.3" x14ac:dyDescent="0.4">
+      <c r="A35" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B35" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="30">
+      <c r="C35" s="47">
         <v>2</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E34" s="15">
-        <v>771</v>
-      </c>
-      <c r="F34" s="2" t="s">
+      <c r="D35" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="G34" s="9"/>
-      <c r="H34" s="11" t="s">
+      <c r="E35" s="32">
+        <v>787</v>
+      </c>
+      <c r="F35" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="G35" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="H35" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="70" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
+    <row r="36" spans="1:9" s="55" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A36" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B36" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="30">
+      <c r="C36" s="50">
         <v>2</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D36" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" s="52">
+        <v>793</v>
+      </c>
+      <c r="F36" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="E35" s="15">
-        <v>787</v>
-      </c>
-      <c r="F35" s="2" t="s">
+      <c r="G36" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="H36" s="54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="41" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A37" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="47"/>
+      <c r="D37" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="E37" s="32">
+        <v>827</v>
+      </c>
+      <c r="F37" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="G37" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="H37" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="41" customFormat="1" ht="51.9" x14ac:dyDescent="0.4">
+      <c r="A38" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="47"/>
+      <c r="D38" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="E38" s="32">
+        <v>827</v>
+      </c>
+      <c r="F38" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="G38" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="H35" s="11" t="s">
+      <c r="H38" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="56" x14ac:dyDescent="0.2">
-      <c r="A36" s="10" t="s">
+    <row r="39" spans="1:9" s="41" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A39" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B39" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="30">
-        <v>2</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E36" s="15">
-        <v>793</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G36" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="H36" s="11" t="s">
+      <c r="C39" s="47"/>
+      <c r="D39" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="E39" s="32">
+        <v>840</v>
+      </c>
+      <c r="F39" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="G39" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="H39" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="42" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
+    <row r="40" spans="1:9" s="55" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A40" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B40" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="30"/>
-      <c r="D37" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E37" s="15">
-        <v>827</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H37" s="11" t="s">
+      <c r="C40" s="50"/>
+      <c r="D40" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="E40" s="52">
+        <v>925</v>
+      </c>
+      <c r="F40" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="G40" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="H40" s="54" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="57" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
+      <c r="I40" s="55" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="45" customFormat="1" ht="90" x14ac:dyDescent="0.4">
+      <c r="A41" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B41" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C38" s="30"/>
-      <c r="D38" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E38" s="15">
-        <v>827</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="G38" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="H38" s="11" t="s">
+      <c r="C41" s="46"/>
+      <c r="D41" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="E41" s="38">
+        <v>942</v>
+      </c>
+      <c r="F41" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="G41" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="H41" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="43" x14ac:dyDescent="0.2">
-      <c r="A39" s="10" t="s">
+    <row r="42" spans="1:9" s="55" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A42" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B42" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="C39" s="30"/>
-      <c r="D39" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E39" s="15">
-        <v>840</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G39" s="11" t="s">
+      <c r="C42" s="50"/>
+      <c r="D42" s="51" t="s">
+        <v>147</v>
+      </c>
+      <c r="E42" s="52">
+        <v>942</v>
+      </c>
+      <c r="F42" s="57" t="s">
         <v>146</v>
       </c>
-      <c r="H39" s="11" t="s">
+      <c r="G42" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="H42" s="54" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="42" x14ac:dyDescent="0.2">
-      <c r="A40" s="10" t="s">
+    <row r="43" spans="1:9" s="41" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A43" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B43" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="30"/>
-      <c r="D40" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E40" s="15">
-        <v>925</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H40" s="11" t="s">
+      <c r="C43" s="47"/>
+      <c r="D43" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="E43" s="32">
+        <v>977</v>
+      </c>
+      <c r="F43" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="G43" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="H43" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="84" x14ac:dyDescent="0.2">
-      <c r="A41" s="10" t="s">
+    <row r="44" spans="1:9" s="41" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A44" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B44" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="30"/>
-      <c r="D41" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E41" s="15">
-        <v>942</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="G41" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="H41" s="11" t="s">
+      <c r="C44" s="47"/>
+      <c r="D44" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="E44" s="32">
+        <v>996</v>
+      </c>
+      <c r="F44" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="G44" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="H44" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A42" s="10" t="s">
+    <row r="45" spans="1:9" s="55" customFormat="1" ht="64.3" x14ac:dyDescent="0.4">
+      <c r="A45" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B45" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="30"/>
-      <c r="D42" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E42" s="15">
-        <v>942</v>
-      </c>
-      <c r="F42" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="G42" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="H42" s="11" t="s">
+      <c r="C45" s="50"/>
+      <c r="D45" s="51" t="s">
+        <v>162</v>
+      </c>
+      <c r="E45" s="52">
+        <v>1014</v>
+      </c>
+      <c r="F45" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="G45" s="51" t="s">
+        <v>161</v>
+      </c>
+      <c r="H45" s="54" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="42" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C43" s="30"/>
-      <c r="D43" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E43" s="15">
-        <v>977</v>
-      </c>
-      <c r="F43" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="H43" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="42" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C44" s="30"/>
-      <c r="D44" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E44" s="15">
-        <v>996</v>
-      </c>
-      <c r="F44" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="H44" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="70" x14ac:dyDescent="0.2">
-      <c r="A45" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C45" s="30"/>
-      <c r="D45" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E45" s="15">
-        <v>1014</v>
-      </c>
-      <c r="F45" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="H45" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I45" s="55" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A46" s="1"/>
       <c r="B46" s="3"/>
-      <c r="C46" s="30"/>
+      <c r="C46" s="15"/>
       <c r="D46" s="2"/>
-      <c r="E46" s="15"/>
+      <c r="E46" s="8"/>
       <c r="F46" s="1"/>
-      <c r="G46" s="9"/>
+      <c r="G46" s="7"/>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A47" s="1"/>
       <c r="B47" s="3"/>
-      <c r="C47" s="30"/>
+      <c r="C47" s="15"/>
       <c r="D47" s="2"/>
-      <c r="E47" s="15"/>
+      <c r="E47" s="8"/>
       <c r="F47" s="1"/>
-      <c r="G47" s="9"/>
+      <c r="G47" s="7"/>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A48" s="1"/>
       <c r="B48" s="3"/>
-      <c r="C48" s="30"/>
+      <c r="C48" s="15"/>
       <c r="D48" s="2"/>
-      <c r="E48" s="15"/>
+      <c r="E48" s="8"/>
       <c r="F48" s="1"/>
-      <c r="G48" s="9"/>
+      <c r="G48" s="7"/>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A49" s="1"/>
       <c r="B49" s="3"/>
-      <c r="C49" s="30"/>
+      <c r="C49" s="15"/>
       <c r="D49" s="2"/>
-      <c r="E49" s="15"/>
+      <c r="E49" s="8"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="9"/>
+      <c r="G49" s="7"/>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A50" s="1"/>
       <c r="B50" s="3"/>
-      <c r="C50" s="30"/>
+      <c r="C50" s="15"/>
       <c r="D50" s="2"/>
-      <c r="E50" s="15"/>
+      <c r="E50" s="8"/>
       <c r="F50" s="1"/>
-      <c r="G50" s="9"/>
+      <c r="G50" s="7"/>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A51" s="1"/>
       <c r="B51" s="3"/>
-      <c r="C51" s="30"/>
+      <c r="C51" s="15"/>
       <c r="D51" s="2"/>
-      <c r="E51" s="15"/>
+      <c r="E51" s="8"/>
       <c r="F51" s="1"/>
-      <c r="G51" s="9"/>
+      <c r="G51" s="7"/>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A52" s="1"/>
       <c r="B52" s="3"/>
-      <c r="C52" s="30"/>
+      <c r="C52" s="15"/>
       <c r="D52" s="2"/>
-      <c r="E52" s="15"/>
+      <c r="E52" s="8"/>
       <c r="F52" s="1"/>
-      <c r="G52" s="9"/>
+      <c r="G52" s="7"/>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A53" s="1"/>
       <c r="B53" s="3"/>
-      <c r="C53" s="30"/>
+      <c r="C53" s="15"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="15"/>
+      <c r="E53" s="8"/>
       <c r="F53" s="1"/>
-      <c r="G53" s="9"/>
+      <c r="G53" s="7"/>
       <c r="H53" s="1"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A54" s="1"/>
       <c r="B54" s="3"/>
-      <c r="C54" s="30"/>
+      <c r="C54" s="15"/>
       <c r="D54" s="2"/>
-      <c r="E54" s="15"/>
+      <c r="E54" s="8"/>
       <c r="F54" s="1"/>
-      <c r="G54" s="9"/>
+      <c r="G54" s="7"/>
       <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A55" s="1"/>
       <c r="B55" s="3"/>
-      <c r="C55" s="30"/>
+      <c r="C55" s="15"/>
       <c r="D55" s="2"/>
-      <c r="E55" s="15"/>
+      <c r="E55" s="8"/>
       <c r="F55" s="1"/>
-      <c r="G55" s="9"/>
+      <c r="G55" s="7"/>
       <c r="H55" s="1"/>
     </row>
   </sheetData>
@@ -4061,257 +4192,257 @@
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="115.5" customWidth="1"/>
+    <col min="1" max="1" width="115.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>25</v>
       </c>
@@ -4330,19 +4461,19 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Updated mACM based on public comments
Updated final public comments for mACM, including updating the use case to use mCSD and updating diagrams.
</commit_message>
<xml_diff>
--- a/FHIR-R4/ITI_Comment_Form-mACM-Felhofer.xlsx
+++ b/FHIR-R4/ITI_Comment_Form-mACM-Felhofer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\IT-Infrastructure\FHIR-R4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E642D6-8F32-4FEB-BFE1-705E03D2D301}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6B3D37-E5AD-41ED-84F0-5178AC2916BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4886" windowWidth="17906" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="32477" windowHeight="16012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comment Form" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="166">
   <si>
     <t>Priority</t>
   </si>
@@ -2335,7 +2335,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2344,19 +2344,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2455,7 +2443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2512,116 +2500,69 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2963,8 +2904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2980,31 +2921,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.45" x14ac:dyDescent="0.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
     </row>
     <row r="2" spans="1:10" ht="269.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="1:10" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
@@ -3034,33 +2975,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="25" customFormat="1" ht="38.6" x14ac:dyDescent="0.4">
-      <c r="A6" s="22" t="s">
+    <row r="6" spans="1:10" s="20" customFormat="1" ht="38.6" x14ac:dyDescent="0.4">
+      <c r="A6" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="17">
         <v>293</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="21" customFormat="1" ht="115.75" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" s="20" customFormat="1" ht="115.75" x14ac:dyDescent="0.4">
       <c r="A7" s="17" t="s">
         <v>63</v>
       </c>
@@ -3079,99 +3020,99 @@
       <c r="F7" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="35" t="s">
         <v>65</v>
       </c>
       <c r="H7" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="25" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A8" s="22" t="s">
+    <row r="8" spans="1:10" s="20" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A8" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="21">
         <v>1</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="19">
         <v>4</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="19">
         <v>325</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="25" customFormat="1" ht="102.9" x14ac:dyDescent="0.4">
-      <c r="A9" s="22" t="s">
+    <row r="9" spans="1:10" s="20" customFormat="1" ht="102.9" x14ac:dyDescent="0.4">
+      <c r="A9" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="21">
         <v>1</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="19">
         <v>371</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="25" customFormat="1" ht="102.9" x14ac:dyDescent="0.4">
-      <c r="A10" s="22" t="s">
+    <row r="10" spans="1:10" s="20" customFormat="1" ht="102.9" x14ac:dyDescent="0.4">
+      <c r="A10" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="21">
         <v>1</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="22">
         <v>379</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="21" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" s="20" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
       <c r="A11" s="17" t="s">
         <v>63</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="21">
         <v>1</v>
       </c>
       <c r="D11" s="19" t="s">
@@ -3183,316 +3124,316 @@
       <c r="F11" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="36" t="s">
         <v>73</v>
       </c>
       <c r="H11" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="25" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A12" s="22" t="s">
+    <row r="12" spans="1:10" s="20" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A12" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="21">
         <v>1</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="19">
         <v>411</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="25" customFormat="1" ht="25.75" x14ac:dyDescent="0.4">
-      <c r="A13" s="22" t="s">
+    <row r="13" spans="1:10" s="20" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A13" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="21">
         <v>1</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="19">
         <v>424</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="G13" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="H13" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="25" customFormat="1" ht="141.44999999999999" x14ac:dyDescent="0.4">
-      <c r="A14" s="22" t="s">
+    <row r="14" spans="1:10" s="20" customFormat="1" ht="141.44999999999999" x14ac:dyDescent="0.4">
+      <c r="A14" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="21">
         <v>1</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="19">
         <v>453</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="F14" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="G14" s="24" t="s">
+      <c r="G14" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="H14" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="25" customFormat="1" ht="90" x14ac:dyDescent="0.4">
-      <c r="A15" s="22" t="s">
+    <row r="15" spans="1:10" s="20" customFormat="1" ht="90" x14ac:dyDescent="0.4">
+      <c r="A15" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="21">
         <v>1</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="19">
         <v>480</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F15" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="25" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A16" s="22" t="s">
+    <row r="16" spans="1:10" s="20" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="21">
         <v>1</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="19">
         <v>500</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="G16" s="24" t="s">
+      <c r="G16" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="25" customFormat="1" ht="102.9" x14ac:dyDescent="0.4">
-      <c r="A17" s="22" t="s">
+    <row r="17" spans="1:8" s="20" customFormat="1" ht="102.9" x14ac:dyDescent="0.4">
+      <c r="A17" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="21">
         <v>1</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E17" s="19">
         <v>500</v>
       </c>
-      <c r="F17" s="24" t="s">
+      <c r="F17" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="G17" s="24" t="s">
+      <c r="G17" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="H17" s="24" t="s">
+      <c r="H17" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="37" customFormat="1" ht="102.9" x14ac:dyDescent="0.4">
-      <c r="A18" s="33" t="s">
+    <row r="18" spans="1:8" s="28" customFormat="1" ht="102.9" x14ac:dyDescent="0.4">
+      <c r="A18" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="25">
         <v>1</v>
       </c>
-      <c r="D18" s="35">
+      <c r="D18" s="26">
         <v>42.5</v>
       </c>
-      <c r="E18" s="36">
+      <c r="E18" s="27">
         <v>556</v>
       </c>
-      <c r="F18" s="35" t="s">
+      <c r="F18" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="G18" s="35" t="s">
+      <c r="G18" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="H18" s="35" t="s">
+      <c r="H18" s="26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="25" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A19" s="22" t="s">
+    <row r="19" spans="1:8" s="20" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A19" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="21">
         <v>1</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="23">
         <v>563</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F19" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="G19" s="32" t="s">
+      <c r="G19" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="25" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A20" s="22" t="s">
+    <row r="20" spans="1:8" s="20" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A20" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="21">
         <v>1</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="23">
         <v>566</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F20" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="G20" s="24" t="s">
+      <c r="G20" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="H20" s="24" t="s">
+      <c r="H20" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="25" customFormat="1" ht="141" x14ac:dyDescent="0.4">
-      <c r="A21" s="22" t="s">
+    <row r="21" spans="1:8" s="20" customFormat="1" ht="141" x14ac:dyDescent="0.4">
+      <c r="A21" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="21">
         <v>1</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="D21" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="23">
         <v>573</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="G21" s="24" t="s">
+      <c r="G21" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="H21" s="24" t="s">
+      <c r="H21" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="25" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A22" s="22" t="s">
+    <row r="22" spans="1:8" s="20" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A22" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C22" s="21">
         <v>1</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D22" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="23">
         <v>577</v>
       </c>
-      <c r="F22" s="24" t="s">
+      <c r="F22" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="G22" s="24" t="s">
+      <c r="G22" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="H22" s="24" t="s">
+      <c r="H22" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="21" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" s="20" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
       <c r="A23" s="17" t="s">
         <v>63</v>
       </c>
       <c r="B23" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="21">
         <v>1</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="23">
         <v>585</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="F23" s="20" t="s">
         <v>104</v>
       </c>
       <c r="G23" s="19" t="s">
@@ -3502,555 +3443,555 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="41" customFormat="1" ht="84.9" x14ac:dyDescent="0.4">
-      <c r="A24" s="22" t="s">
+    <row r="24" spans="1:8" s="31" customFormat="1" ht="84.9" x14ac:dyDescent="0.4">
+      <c r="A24" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="26">
+      <c r="C24" s="21">
         <v>1</v>
       </c>
-      <c r="D24" s="39" t="s">
+      <c r="D24" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="23">
         <v>626</v>
       </c>
-      <c r="F24" s="39" t="s">
+      <c r="F24" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G24" s="40" t="s">
+      <c r="G24" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="H24" s="24" t="s">
+      <c r="H24" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="41" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A25" s="22" t="s">
+    <row r="25" spans="1:8" s="31" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A25" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="26">
+      <c r="C25" s="21">
         <v>1</v>
       </c>
-      <c r="D25" s="39" t="s">
+      <c r="D25" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="E25" s="32">
+      <c r="E25" s="23">
         <v>633</v>
       </c>
-      <c r="F25" s="39" t="s">
+      <c r="F25" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="G25" s="42"/>
-      <c r="H25" s="24" t="s">
+      <c r="G25" s="32"/>
+      <c r="H25" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="45" customFormat="1" ht="77.150000000000006" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" s="31" customFormat="1" ht="77.150000000000006" x14ac:dyDescent="0.4">
       <c r="A26" s="17" t="s">
         <v>63</v>
       </c>
       <c r="B26" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="28">
+      <c r="C26" s="21">
         <v>1</v>
       </c>
-      <c r="D26" s="43" t="s">
+      <c r="D26" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="E26" s="38">
+      <c r="E26" s="23">
         <v>640</v>
       </c>
-      <c r="F26" s="43" t="s">
+      <c r="F26" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="G26" s="44"/>
+      <c r="G26" s="32"/>
       <c r="H26" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="41" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A27" s="22" t="s">
+    <row r="27" spans="1:8" s="31" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A27" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="21">
         <v>1</v>
       </c>
-      <c r="D27" s="39" t="s">
+      <c r="D27" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="E27" s="32" t="s">
+      <c r="E27" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="F27" s="39" t="s">
+      <c r="F27" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="G27" s="42" t="s">
+      <c r="G27" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="H27" s="24" t="s">
+      <c r="H27" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="45" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" s="31" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
       <c r="A28" s="17" t="s">
         <v>63</v>
       </c>
       <c r="B28" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="46">
+      <c r="C28" s="33">
         <v>2</v>
       </c>
-      <c r="D28" s="43" t="s">
+      <c r="D28" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="E28" s="38" t="s">
+      <c r="E28" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="F28" s="43" t="s">
+      <c r="F28" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="G28" s="44" t="s">
+      <c r="G28" s="32" t="s">
         <v>131</v>
       </c>
       <c r="H28" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="41" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A29" s="22" t="s">
+    <row r="29" spans="1:8" s="31" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A29" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="47"/>
-      <c r="D29" s="39" t="s">
+      <c r="C29" s="33"/>
+      <c r="D29" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="E29" s="32">
+      <c r="E29" s="23">
         <v>699</v>
       </c>
-      <c r="F29" s="39" t="s">
+      <c r="F29" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="G29" s="39" t="s">
+      <c r="G29" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="H29" s="24" t="s">
+      <c r="H29" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="41" customFormat="1" ht="56.6" x14ac:dyDescent="0.4">
-      <c r="A30" s="22" t="s">
+    <row r="30" spans="1:8" s="31" customFormat="1" ht="56.6" x14ac:dyDescent="0.4">
+      <c r="A30" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="47">
+      <c r="C30" s="33">
         <v>2</v>
       </c>
-      <c r="D30" s="39" t="s">
+      <c r="D30" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="E30" s="32">
+      <c r="E30" s="23">
         <v>760</v>
       </c>
-      <c r="F30" s="39" t="s">
+      <c r="F30" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="G30" s="40" t="s">
+      <c r="G30" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="H30" s="24" t="s">
+      <c r="H30" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="41" customFormat="1" ht="70.75" x14ac:dyDescent="0.4">
-      <c r="A31" s="22" t="s">
+    <row r="31" spans="1:8" s="31" customFormat="1" ht="70.75" x14ac:dyDescent="0.4">
+      <c r="A31" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="47">
+      <c r="C31" s="33">
         <v>2</v>
       </c>
-      <c r="D31" s="39" t="s">
+      <c r="D31" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="E31" s="32">
+      <c r="E31" s="23">
         <v>760</v>
       </c>
-      <c r="F31" s="39" t="s">
+      <c r="F31" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="G31" s="40" t="s">
+      <c r="G31" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="H31" s="24" t="s">
+      <c r="H31" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="41" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A32" s="22" t="s">
+    <row r="32" spans="1:8" s="31" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A32" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="47">
+      <c r="C32" s="33">
         <v>2</v>
       </c>
-      <c r="D32" s="39" t="s">
+      <c r="D32" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="E32" s="32">
+      <c r="E32" s="23">
         <v>760</v>
       </c>
-      <c r="F32" s="39" t="s">
+      <c r="F32" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="G32" s="40" t="s">
+      <c r="G32" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="H32" s="24" t="s">
+      <c r="H32" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="41" customFormat="1" ht="179.6" x14ac:dyDescent="0.4">
-      <c r="A33" s="22" t="s">
+    <row r="33" spans="1:9" s="31" customFormat="1" ht="179.6" x14ac:dyDescent="0.4">
+      <c r="A33" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="47">
+      <c r="C33" s="33">
         <v>2</v>
       </c>
-      <c r="D33" s="39" t="s">
+      <c r="D33" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E33" s="23">
         <v>760</v>
       </c>
-      <c r="F33" s="39" t="s">
+      <c r="F33" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="G33" s="39" t="s">
+      <c r="G33" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="H33" s="24" t="s">
+      <c r="H33" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="41" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A34" s="22" t="s">
+    <row r="34" spans="1:9" s="31" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A34" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="47">
+      <c r="C34" s="33">
         <v>2</v>
       </c>
-      <c r="D34" s="39" t="s">
+      <c r="D34" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="E34" s="32">
+      <c r="E34" s="23">
         <v>771</v>
       </c>
-      <c r="F34" s="39" t="s">
+      <c r="F34" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="G34" s="48"/>
-      <c r="H34" s="24" t="s">
+      <c r="G34" s="34"/>
+      <c r="H34" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="41" customFormat="1" ht="64.3" x14ac:dyDescent="0.4">
-      <c r="A35" s="22" t="s">
+    <row r="35" spans="1:9" s="31" customFormat="1" ht="64.3" x14ac:dyDescent="0.4">
+      <c r="A35" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="47">
+      <c r="C35" s="33">
         <v>2</v>
       </c>
-      <c r="D35" s="39" t="s">
+      <c r="D35" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="E35" s="32">
+      <c r="E35" s="23">
         <v>787</v>
       </c>
-      <c r="F35" s="39" t="s">
+      <c r="F35" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="G35" s="39" t="s">
+      <c r="G35" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="H35" s="24" t="s">
+      <c r="H35" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="55" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A36" s="49" t="s">
+    <row r="36" spans="1:9" s="31" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A36" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="49" t="s">
+      <c r="B36" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="50">
+      <c r="C36" s="33">
         <v>2</v>
       </c>
-      <c r="D36" s="51" t="s">
+      <c r="D36" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="E36" s="52">
+      <c r="E36" s="23">
         <v>793</v>
       </c>
-      <c r="F36" s="51" t="s">
+      <c r="F36" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="G36" s="53" t="s">
+      <c r="G36" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="H36" s="54" t="s">
+      <c r="H36" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="41" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A37" s="22" t="s">
+    <row r="37" spans="1:9" s="31" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A37" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="47"/>
-      <c r="D37" s="39" t="s">
+      <c r="C37" s="33"/>
+      <c r="D37" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="E37" s="32">
+      <c r="E37" s="23">
         <v>827</v>
       </c>
-      <c r="F37" s="39" t="s">
+      <c r="F37" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="G37" s="39" t="s">
+      <c r="G37" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="H37" s="24" t="s">
+      <c r="H37" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="41" customFormat="1" ht="51.9" x14ac:dyDescent="0.4">
-      <c r="A38" s="22" t="s">
+    <row r="38" spans="1:9" s="31" customFormat="1" ht="51.9" x14ac:dyDescent="0.4">
+      <c r="A38" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C38" s="47"/>
-      <c r="D38" s="39" t="s">
+      <c r="C38" s="33"/>
+      <c r="D38" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="E38" s="32">
+      <c r="E38" s="23">
         <v>827</v>
       </c>
-      <c r="F38" s="39" t="s">
+      <c r="F38" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="G38" s="24" t="s">
+      <c r="G38" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="H38" s="24" t="s">
+      <c r="H38" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="41" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A39" s="22" t="s">
+    <row r="39" spans="1:9" s="31" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A39" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C39" s="47"/>
-      <c r="D39" s="39" t="s">
+      <c r="C39" s="33"/>
+      <c r="D39" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="E39" s="32">
+      <c r="E39" s="23">
         <v>840</v>
       </c>
-      <c r="F39" s="39" t="s">
+      <c r="F39" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="G39" s="24" t="s">
+      <c r="G39" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="H39" s="24" t="s">
+      <c r="H39" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="55" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A40" s="49" t="s">
+    <row r="40" spans="1:9" s="31" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A40" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="49" t="s">
+      <c r="B40" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="50"/>
-      <c r="D40" s="51" t="s">
+      <c r="C40" s="33"/>
+      <c r="D40" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="E40" s="52">
+      <c r="E40" s="23">
         <v>925</v>
       </c>
-      <c r="F40" s="51" t="s">
+      <c r="F40" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="G40" s="51" t="s">
+      <c r="G40" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="H40" s="54" t="s">
+      <c r="H40" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I40" s="55" t="s">
+      <c r="I40" s="31" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="45" customFormat="1" ht="90" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:9" s="31" customFormat="1" ht="90" x14ac:dyDescent="0.4">
       <c r="A41" s="17" t="s">
         <v>63</v>
       </c>
       <c r="B41" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="46"/>
-      <c r="D41" s="43" t="s">
+      <c r="C41" s="33"/>
+      <c r="D41" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="E41" s="38">
+      <c r="E41" s="23">
         <v>942</v>
       </c>
-      <c r="F41" s="43" t="s">
+      <c r="F41" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="G41" s="56" t="s">
+      <c r="G41" s="37" t="s">
         <v>148</v>
       </c>
       <c r="H41" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="55" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A42" s="49" t="s">
+    <row r="42" spans="1:9" s="31" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A42" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B42" s="49" t="s">
+      <c r="B42" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="50"/>
-      <c r="D42" s="51" t="s">
+      <c r="C42" s="33"/>
+      <c r="D42" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="E42" s="52">
+      <c r="E42" s="23">
         <v>942</v>
       </c>
-      <c r="F42" s="57" t="s">
+      <c r="F42" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="G42" s="58" t="s">
+      <c r="G42" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="H42" s="54" t="s">
+      <c r="H42" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="41" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A43" s="22" t="s">
+    <row r="43" spans="1:9" s="31" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A43" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="47"/>
-      <c r="D43" s="39" t="s">
+      <c r="C43" s="33"/>
+      <c r="D43" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="E43" s="32">
+      <c r="E43" s="23">
         <v>977</v>
       </c>
-      <c r="F43" s="39" t="s">
+      <c r="F43" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="G43" s="39" t="s">
+      <c r="G43" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="H43" s="24" t="s">
+      <c r="H43" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="41" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A44" s="22" t="s">
+    <row r="44" spans="1:9" s="31" customFormat="1" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A44" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="47"/>
-      <c r="D44" s="39" t="s">
+      <c r="C44" s="33"/>
+      <c r="D44" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="E44" s="32">
+      <c r="E44" s="23">
         <v>996</v>
       </c>
-      <c r="F44" s="39" t="s">
+      <c r="F44" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="G44" s="39" t="s">
+      <c r="G44" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="H44" s="24" t="s">
+      <c r="H44" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="55" customFormat="1" ht="64.3" x14ac:dyDescent="0.4">
-      <c r="A45" s="49" t="s">
+    <row r="45" spans="1:9" s="31" customFormat="1" ht="64.3" x14ac:dyDescent="0.4">
+      <c r="A45" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="49" t="s">
+      <c r="B45" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="50"/>
-      <c r="D45" s="51" t="s">
+      <c r="C45" s="33"/>
+      <c r="D45" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="E45" s="52">
+      <c r="E45" s="23">
         <v>1014</v>
       </c>
-      <c r="F45" s="51" t="s">
+      <c r="F45" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="G45" s="51" t="s">
+      <c r="G45" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="H45" s="54" t="s">
+      <c r="H45" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I45" s="55" t="s">
+      <c r="I45" s="31" t="s">
         <v>165</v>
       </c>
     </row>

</xml_diff>